<commit_message>
a score change for VGGT 16-8b (Kazakhstan)
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/NKT-VGGT16/2017-NKT-VGGT-16.8-16.9.xlsx
+++ b/Simple_XLS_Importer/data/NKT-VGGT16/2017-NKT-VGGT-16.8-16.9.xlsx
@@ -17,16 +17,11 @@
     <sheet name="Legend" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="164">
   <si>
     <t>Bangladesh</t>
   </si>
@@ -544,9 +539,6 @@
   </si>
   <si>
     <t>According to the LARR Act, 2013 an Expert Group must appraise the Social Impact Assessment and report on whether “land proposed to be acquired is the absolute bare-minimum extent needed for the project and whether there are no other less displacing options available.” (Sec. 7(5), LARR Act). Section 8(2) requires the appropriate Government to examine the report of the Collector on Expert Group on Social Impact Assessment and, after consider the reports, recommend such area for acquisition which would ensure minimum displace of people, minimum disturbance and minimum adverse impact on the individuals affected (Sec. 8(2), LARR Act). Section 39 provides that the Collector must "as far, as possible, not displace any family which has already been displaced by the appropriated Government, and, if so, shall pay additional compensation..."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pursuant to article 62(2) of the 2011 Law on State-owned Property, "Compulsory acquisition of the parcel of land or other real estate in connection with withdrawal of the parcel of land for the state needs in the presence of different (alternative) way of satisfaction of the state needs is not allowed." The score on this indicator is “partial” because, while the government is only allowed to expropriate land if no other available alternatives exist, it is unclear from this provision whether the government is necessarily obligated to avoid or minimize involuntary resettlement in every case. </t>
   </si>
   <si>
     <t xml:space="preserve">The government can only require indigenous communities to relocate from their lands where relocation "is considered necessary as an exceptional measure" (Sec. 7(c), Indigenous Peoples Rights Act, 1997). (Section 7 (c) Indigenous People’s Right Act). The answer is "partial" because the government is only obliged to minimize or avoid forced evictions in cases involving indigenous land. </t>
@@ -692,7 +684,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -717,6 +709,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -746,7 +744,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2362">
+  <cellStyleXfs count="2363">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3109,8 +3107,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3167,8 +3166,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="2362" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="2362" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2362">
+  <cellStyles count="2363">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -5529,6 +5532,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="2361" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2248"/>
+    <cellStyle name="Normal 3" xfId="2362"/>
     <cellStyle name="Título 2" xfId="2213" builtinId="17"/>
     <cellStyle name="Título 2 2" xfId="2249"/>
   </cellStyles>
@@ -5588,7 +5592,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5623,7 +5627,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5834,8 +5838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H946"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A253" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D265" sqref="D265:E265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5867,7 +5871,7 @@
     </row>
     <row r="2" spans="1:8" s="13" customFormat="1" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>50</v>
@@ -5879,7 +5883,7 @@
         <v>40</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
@@ -5887,7 +5891,7 @@
     </row>
     <row r="3" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>6</v>
@@ -5899,12 +5903,12 @@
         <v>40</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>51</v>
@@ -5916,12 +5920,12 @@
         <v>40</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>0</v>
@@ -5933,12 +5937,12 @@
         <v>40</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>52</v>
@@ -5950,12 +5954,12 @@
         <v>40</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>53</v>
@@ -5967,12 +5971,12 @@
         <v>40</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>54</v>
@@ -5984,12 +5988,12 @@
         <v>40</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>7</v>
@@ -6001,12 +6005,12 @@
         <v>40</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>8</v>
@@ -6018,12 +6022,12 @@
         <v>40</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>9</v>
@@ -6035,12 +6039,12 @@
         <v>40</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>10</v>
@@ -6057,7 +6061,7 @@
     </row>
     <row r="13" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>55</v>
@@ -6069,12 +6073,12 @@
         <v>40</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>56</v>
@@ -6086,12 +6090,12 @@
         <v>40</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>11</v>
@@ -6103,12 +6107,12 @@
         <v>40</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>34</v>
@@ -6120,12 +6124,12 @@
         <v>40</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>33</v>
@@ -6137,12 +6141,12 @@
         <v>40</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>13</v>
@@ -6159,7 +6163,7 @@
     </row>
     <row r="19" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>12</v>
@@ -6171,12 +6175,12 @@
         <v>40</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>14</v>
@@ -6188,12 +6192,12 @@
         <v>40</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>32</v>
@@ -6205,12 +6209,12 @@
         <v>40</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>57</v>
@@ -6222,12 +6226,12 @@
         <v>38</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>58</v>
@@ -6239,12 +6243,12 @@
         <v>40</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>15</v>
@@ -6256,12 +6260,12 @@
         <v>40</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>59</v>
@@ -6273,12 +6277,12 @@
         <v>40</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>16</v>
@@ -6290,12 +6294,12 @@
         <v>40</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>17</v>
@@ -6307,12 +6311,12 @@
         <v>40</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>60</v>
@@ -6324,12 +6328,12 @@
         <v>40</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>61</v>
@@ -6341,12 +6345,12 @@
         <v>40</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>18</v>
@@ -6358,12 +6362,12 @@
         <v>40</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B31" s="14" t="s">
         <v>62</v>
@@ -6375,12 +6379,12 @@
         <v>40</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B32" s="14" t="s">
         <v>19</v>
@@ -6392,12 +6396,12 @@
         <v>40</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B33" s="14" t="s">
         <v>63</v>
@@ -6409,12 +6413,12 @@
         <v>40</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>64</v>
@@ -6426,12 +6430,12 @@
         <v>40</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B35" s="14" t="s">
         <v>65</v>
@@ -6443,12 +6447,12 @@
         <v>40</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>20</v>
@@ -6465,7 +6469,7 @@
     </row>
     <row r="37" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>21</v>
@@ -6477,12 +6481,12 @@
         <v>40</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>22</v>
@@ -6494,12 +6498,12 @@
         <v>40</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B39" s="14" t="s">
         <v>31</v>
@@ -6511,12 +6515,12 @@
         <v>40</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B40" s="14" t="s">
         <v>66</v>
@@ -6528,12 +6532,12 @@
         <v>40</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B41" s="14" t="s">
         <v>23</v>
@@ -6545,12 +6549,12 @@
         <v>40</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>68</v>
@@ -6562,12 +6566,12 @@
         <v>40</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B43" s="14" t="s">
         <v>24</v>
@@ -6579,12 +6583,12 @@
         <v>40</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B44" s="14" t="s">
         <v>25</v>
@@ -6596,12 +6600,12 @@
         <v>40</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>26</v>
@@ -6613,12 +6617,12 @@
         <v>40</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>67</v>
@@ -6630,12 +6634,12 @@
         <v>40</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>27</v>
@@ -6647,12 +6651,12 @@
         <v>40</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B48" s="14" t="s">
         <v>28</v>
@@ -6669,7 +6673,7 @@
     </row>
     <row r="49" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B49" s="14" t="s">
         <v>29</v>
@@ -6686,7 +6690,7 @@
     </row>
     <row r="50" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B50" s="14" t="s">
         <v>30</v>
@@ -6703,7 +6707,7 @@
     </row>
     <row r="51" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B51" s="14" t="s">
         <v>50</v>
@@ -6720,7 +6724,7 @@
     </row>
     <row r="52" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B52" s="14" t="s">
         <v>6</v>
@@ -6737,7 +6741,7 @@
     </row>
     <row r="53" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>51</v>
@@ -6754,7 +6758,7 @@
     </row>
     <row r="54" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B54" s="14" t="s">
         <v>0</v>
@@ -6771,7 +6775,7 @@
     </row>
     <row r="55" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B55" s="14" t="s">
         <v>52</v>
@@ -6788,7 +6792,7 @@
     </row>
     <row r="56" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>53</v>
@@ -6805,7 +6809,7 @@
     </row>
     <row r="57" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B57" s="14" t="s">
         <v>54</v>
@@ -6822,7 +6826,7 @@
     </row>
     <row r="58" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>7</v>
@@ -6839,7 +6843,7 @@
     </row>
     <row r="59" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>8</v>
@@ -6856,7 +6860,7 @@
     </row>
     <row r="60" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B60" s="14" t="s">
         <v>9</v>
@@ -6873,7 +6877,7 @@
     </row>
     <row r="61" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B61" s="14" t="s">
         <v>10</v>
@@ -6890,7 +6894,7 @@
     </row>
     <row r="62" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B62" s="14" t="s">
         <v>55</v>
@@ -6907,7 +6911,7 @@
     </row>
     <row r="63" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B63" s="14" t="s">
         <v>56</v>
@@ -6924,7 +6928,7 @@
     </row>
     <row r="64" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B64" s="14" t="s">
         <v>11</v>
@@ -6941,7 +6945,7 @@
     </row>
     <row r="65" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B65" s="14" t="s">
         <v>34</v>
@@ -6958,7 +6962,7 @@
     </row>
     <row r="66" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B66" s="14" t="s">
         <v>33</v>
@@ -6975,7 +6979,7 @@
     </row>
     <row r="67" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B67" s="14" t="s">
         <v>13</v>
@@ -6992,7 +6996,7 @@
     </row>
     <row r="68" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B68" s="14" t="s">
         <v>12</v>
@@ -7009,7 +7013,7 @@
     </row>
     <row r="69" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B69" s="14" t="s">
         <v>14</v>
@@ -7026,7 +7030,7 @@
     </row>
     <row r="70" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B70" s="14" t="s">
         <v>32</v>
@@ -7043,7 +7047,7 @@
     </row>
     <row r="71" spans="1:5" s="13" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B71" s="14" t="s">
         <v>57</v>
@@ -7055,12 +7059,12 @@
         <v>38</v>
       </c>
       <c r="E71" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B72" s="14" t="s">
         <v>58</v>
@@ -7077,7 +7081,7 @@
     </row>
     <row r="73" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B73" s="14" t="s">
         <v>15</v>
@@ -7094,7 +7098,7 @@
     </row>
     <row r="74" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B74" s="14" t="s">
         <v>59</v>
@@ -7111,7 +7115,7 @@
     </row>
     <row r="75" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B75" s="14" t="s">
         <v>16</v>
@@ -7128,7 +7132,7 @@
     </row>
     <row r="76" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B76" s="14" t="s">
         <v>17</v>
@@ -7145,7 +7149,7 @@
     </row>
     <row r="77" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B77" s="14" t="s">
         <v>60</v>
@@ -7162,7 +7166,7 @@
     </row>
     <row r="78" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B78" s="14" t="s">
         <v>61</v>
@@ -7179,7 +7183,7 @@
     </row>
     <row r="79" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B79" s="14" t="s">
         <v>18</v>
@@ -7196,7 +7200,7 @@
     </row>
     <row r="80" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B80" s="14" t="s">
         <v>62</v>
@@ -7208,12 +7212,12 @@
         <v>39</v>
       </c>
       <c r="E80" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B81" s="14" t="s">
         <v>19</v>
@@ -7230,7 +7234,7 @@
     </row>
     <row r="82" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B82" s="14" t="s">
         <v>63</v>
@@ -7247,7 +7251,7 @@
     </row>
     <row r="83" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B83" s="14" t="s">
         <v>64</v>
@@ -7264,7 +7268,7 @@
     </row>
     <row r="84" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B84" s="14" t="s">
         <v>65</v>
@@ -7281,7 +7285,7 @@
     </row>
     <row r="85" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B85" s="14" t="s">
         <v>20</v>
@@ -7298,7 +7302,7 @@
     </row>
     <row r="86" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B86" s="14" t="s">
         <v>21</v>
@@ -7315,7 +7319,7 @@
     </row>
     <row r="87" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B87" s="14" t="s">
         <v>22</v>
@@ -7332,7 +7336,7 @@
     </row>
     <row r="88" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B88" s="14" t="s">
         <v>31</v>
@@ -7349,7 +7353,7 @@
     </row>
     <row r="89" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B89" s="14" t="s">
         <v>66</v>
@@ -7366,7 +7370,7 @@
     </row>
     <row r="90" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B90" s="14" t="s">
         <v>23</v>
@@ -7383,7 +7387,7 @@
     </row>
     <row r="91" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B91" s="14" t="s">
         <v>68</v>
@@ -7400,7 +7404,7 @@
     </row>
     <row r="92" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B92" s="14" t="s">
         <v>24</v>
@@ -7417,7 +7421,7 @@
     </row>
     <row r="93" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B93" s="14" t="s">
         <v>25</v>
@@ -7434,7 +7438,7 @@
     </row>
     <row r="94" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B94" s="14" t="s">
         <v>26</v>
@@ -7451,7 +7455,7 @@
     </row>
     <row r="95" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B95" s="14" t="s">
         <v>67</v>
@@ -7468,7 +7472,7 @@
     </row>
     <row r="96" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B96" s="14" t="s">
         <v>27</v>
@@ -7485,7 +7489,7 @@
     </row>
     <row r="97" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B97" s="14" t="s">
         <v>28</v>
@@ -7502,7 +7506,7 @@
     </row>
     <row r="98" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B98" s="14" t="s">
         <v>29</v>
@@ -7519,7 +7523,7 @@
     </row>
     <row r="99" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B99" s="14" t="s">
         <v>30</v>
@@ -7536,7 +7540,7 @@
     </row>
     <row r="100" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B100" s="14" t="s">
         <v>50</v>
@@ -7553,7 +7557,7 @@
     </row>
     <row r="101" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B101" s="14" t="s">
         <v>6</v>
@@ -7570,7 +7574,7 @@
     </row>
     <row r="102" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B102" s="14" t="s">
         <v>51</v>
@@ -7587,7 +7591,7 @@
     </row>
     <row r="103" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B103" s="14" t="s">
         <v>0</v>
@@ -7604,7 +7608,7 @@
     </row>
     <row r="104" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B104" s="14" t="s">
         <v>52</v>
@@ -7621,7 +7625,7 @@
     </row>
     <row r="105" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B105" s="14" t="s">
         <v>53</v>
@@ -7638,7 +7642,7 @@
     </row>
     <row r="106" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B106" s="14" t="s">
         <v>54</v>
@@ -7655,7 +7659,7 @@
     </row>
     <row r="107" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B107" s="14" t="s">
         <v>7</v>
@@ -7672,7 +7676,7 @@
     </row>
     <row r="108" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B108" s="14" t="s">
         <v>8</v>
@@ -7689,7 +7693,7 @@
     </row>
     <row r="109" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B109" s="14" t="s">
         <v>9</v>
@@ -7706,7 +7710,7 @@
     </row>
     <row r="110" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B110" s="14" t="s">
         <v>10</v>
@@ -7723,7 +7727,7 @@
     </row>
     <row r="111" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B111" s="14" t="s">
         <v>55</v>
@@ -7740,7 +7744,7 @@
     </row>
     <row r="112" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B112" s="14" t="s">
         <v>56</v>
@@ -7757,7 +7761,7 @@
     </row>
     <row r="113" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B113" s="14" t="s">
         <v>11</v>
@@ -7774,7 +7778,7 @@
     </row>
     <row r="114" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B114" s="14" t="s">
         <v>34</v>
@@ -7791,7 +7795,7 @@
     </row>
     <row r="115" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B115" s="14" t="s">
         <v>33</v>
@@ -7808,7 +7812,7 @@
     </row>
     <row r="116" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B116" s="14" t="s">
         <v>13</v>
@@ -7825,7 +7829,7 @@
     </row>
     <row r="117" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B117" s="14" t="s">
         <v>12</v>
@@ -7842,7 +7846,7 @@
     </row>
     <row r="118" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B118" s="14" t="s">
         <v>14</v>
@@ -7859,7 +7863,7 @@
     </row>
     <row r="119" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B119" s="14" t="s">
         <v>32</v>
@@ -7876,7 +7880,7 @@
     </row>
     <row r="120" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B120" s="14" t="s">
         <v>57</v>
@@ -7888,12 +7892,12 @@
         <v>38</v>
       </c>
       <c r="E120" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="121" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B121" s="14" t="s">
         <v>58</v>
@@ -7910,7 +7914,7 @@
     </row>
     <row r="122" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B122" s="14" t="s">
         <v>15</v>
@@ -7927,7 +7931,7 @@
     </row>
     <row r="123" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B123" s="14" t="s">
         <v>59</v>
@@ -7944,7 +7948,7 @@
     </row>
     <row r="124" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B124" s="14" t="s">
         <v>16</v>
@@ -7961,7 +7965,7 @@
     </row>
     <row r="125" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B125" s="14" t="s">
         <v>17</v>
@@ -7978,7 +7982,7 @@
     </row>
     <row r="126" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B126" s="14" t="s">
         <v>60</v>
@@ -7995,7 +7999,7 @@
     </row>
     <row r="127" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B127" s="14" t="s">
         <v>61</v>
@@ -8012,7 +8016,7 @@
     </row>
     <row r="128" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B128" s="14" t="s">
         <v>18</v>
@@ -8029,7 +8033,7 @@
     </row>
     <row r="129" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B129" s="14" t="s">
         <v>62</v>
@@ -8041,12 +8045,12 @@
         <v>39</v>
       </c>
       <c r="E129" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="130" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B130" s="14" t="s">
         <v>19</v>
@@ -8063,7 +8067,7 @@
     </row>
     <row r="131" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B131" s="14" t="s">
         <v>63</v>
@@ -8080,7 +8084,7 @@
     </row>
     <row r="132" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B132" s="14" t="s">
         <v>64</v>
@@ -8097,7 +8101,7 @@
     </row>
     <row r="133" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B133" s="14" t="s">
         <v>65</v>
@@ -8114,7 +8118,7 @@
     </row>
     <row r="134" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B134" s="14" t="s">
         <v>20</v>
@@ -8131,7 +8135,7 @@
     </row>
     <row r="135" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B135" s="14" t="s">
         <v>21</v>
@@ -8148,7 +8152,7 @@
     </row>
     <row r="136" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B136" s="14" t="s">
         <v>22</v>
@@ -8165,7 +8169,7 @@
     </row>
     <row r="137" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B137" s="14" t="s">
         <v>31</v>
@@ -8182,7 +8186,7 @@
     </row>
     <row r="138" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B138" s="14" t="s">
         <v>66</v>
@@ -8199,7 +8203,7 @@
     </row>
     <row r="139" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B139" s="14" t="s">
         <v>23</v>
@@ -8216,7 +8220,7 @@
     </row>
     <row r="140" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B140" s="14" t="s">
         <v>68</v>
@@ -8233,7 +8237,7 @@
     </row>
     <row r="141" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B141" s="14" t="s">
         <v>24</v>
@@ -8250,7 +8254,7 @@
     </row>
     <row r="142" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B142" s="14" t="s">
         <v>25</v>
@@ -8267,7 +8271,7 @@
     </row>
     <row r="143" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B143" s="14" t="s">
         <v>26</v>
@@ -8284,7 +8288,7 @@
     </row>
     <row r="144" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B144" s="14" t="s">
         <v>67</v>
@@ -8301,7 +8305,7 @@
     </row>
     <row r="145" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B145" s="14" t="s">
         <v>27</v>
@@ -8318,7 +8322,7 @@
     </row>
     <row r="146" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B146" s="14" t="s">
         <v>28</v>
@@ -8335,7 +8339,7 @@
     </row>
     <row r="147" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B147" s="14" t="s">
         <v>29</v>
@@ -8352,7 +8356,7 @@
     </row>
     <row r="148" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B148" s="14" t="s">
         <v>30</v>
@@ -8721,7 +8725,7 @@
         <v>38</v>
       </c>
       <c r="E169" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="170" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -9554,7 +9558,7 @@
         <v>38</v>
       </c>
       <c r="E218" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="219" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -10349,11 +10353,11 @@
       <c r="C265" s="17">
         <v>2017</v>
       </c>
-      <c r="D265" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="E265" s="16" t="s">
-        <v>151</v>
+      <c r="D265" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E265" s="32" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="266" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -10625,7 +10629,7 @@
         <v>39</v>
       </c>
       <c r="E281" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="282" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -10744,7 +10748,7 @@
         <v>39</v>
       </c>
       <c r="E288" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="289" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -13427,11 +13431,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>